<commit_message>
complete upto advance conditional formating
</commit_message>
<xml_diff>
--- a/Date.xlsx
+++ b/Date.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shahidul\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\AdvanceExcell\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -79,8 +79,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -358,7 +386,7 @@
   <dimension ref="A2:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -371,13 +399,13 @@
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C2" s="1">
         <f ca="1">TODAY()</f>
-        <v>43745</v>
+        <v>43893</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" s="2">
         <f ca="1">NOW()</f>
-        <v>43745.493397453705</v>
+        <v>43893.825182523149</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>